<commit_message>
Version 1.1 de la solapa FacturasPAMI - Agregado de parametros en la query sql de NuevoPami
</commit_message>
<xml_diff>
--- a/DBA/Reportes BI/2021/Facturación/tipo_comprobante.xlsx
+++ b/DBA/Reportes BI/2021/Facturación/tipo_comprobante.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iachenbach\Desktop\FACOEP\DBA\Reportes BI\2021\Facturación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iachenbach\Gobierno de la Ciudad de Buenos Aires\Pablo Alfredo Gadea - Tablero Facoep P BI\FACOEP\DBA\Reportes BI\2021\Facturación\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="21">
   <si>
     <t>FACA2</t>
   </si>
@@ -75,12 +75,24 @@
   </si>
   <si>
     <t>Alimenta a Comprobantes (2)</t>
+  </si>
+  <si>
+    <t>TipoPami</t>
+  </si>
+  <si>
+    <t>Facturado</t>
+  </si>
+  <si>
+    <t>No Aplica</t>
+  </si>
+  <si>
+    <t>Debitos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -122,15 +134,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -158,14 +173,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:E11" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E11"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="Tipo Comprobante" dataDxfId="4"/>
-    <tableColumn id="2" name="Multiplicador" dataDxfId="3"/>
-    <tableColumn id="5" name="Alimenta a Comprobantes (2)" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:F11" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F11"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Tipo Comprobante" dataDxfId="5"/>
+    <tableColumn id="2" name="Multiplicador" dataDxfId="4"/>
+    <tableColumn id="5" name="Alimenta a Comprobantes (2)" dataDxfId="3"/>
     <tableColumn id="3" name="Alimenta a Detalle" dataDxfId="2"/>
     <tableColumn id="4" name="Alimenta a SIF2" dataDxfId="1"/>
+    <tableColumn id="6" name="TipoPami" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -434,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,7 +464,7 @@
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -464,8 +480,11 @@
       <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -481,8 +500,11 @@
       <c r="E2" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -498,8 +520,11 @@
       <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -515,8 +540,11 @@
       <c r="E4" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -532,8 +560,11 @@
       <c r="E5" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -549,8 +580,11 @@
       <c r="E6" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -566,8 +600,11 @@
       <c r="E7" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -583,8 +620,11 @@
       <c r="E8" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -600,8 +640,11 @@
       <c r="E9" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -617,8 +660,11 @@
       <c r="E10" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -633,6 +679,9 @@
       </c>
       <c r="E11" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>